<commit_message>
Other changes to team communication
</commit_message>
<xml_diff>
--- a/Content/Files/meetingMinutes.xlsx
+++ b/Content/Files/meetingMinutes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jozel_000\Documents\RnD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jozel_000\Documents\Portfolio\po\Content\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="23_07_15" sheetId="1" r:id="rId1"/>
@@ -766,6 +766,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,18 +795,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1078,7 +1078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -1093,25 +1093,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
       <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
       <c r="I3" s="2"/>
       <c r="J3" t="s">
         <v>11</v>
@@ -1236,22 +1236,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="12" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1386,22 +1386,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -1486,17 +1486,17 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="13" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="13" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="14" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1537,22 +1537,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
@@ -1673,22 +1673,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -1827,22 +1827,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -1966,7 +1966,7 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1979,22 +1979,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -2124,20 +2124,20 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="4" t="s">
@@ -2271,22 +2271,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2400,22 +2400,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2574,22 +2574,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -2718,22 +2718,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="4" t="s">
@@ -2859,22 +2859,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -2999,22 +2999,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">

</xml_diff>